<commit_message>
Computed some results for the navigation problem
</commit_message>
<xml_diff>
--- a/results/WorldKnown/ValueSum.xlsx
+++ b/results/WorldKnown/ValueSum.xlsx
@@ -1,58 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luker\source\repos\ReinforcementLearning\results\WorldKnown\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C5B6CD-655D-47CC-8AC8-B7D00586B49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="2892" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8994" windowWidth="17280" xWindow="1416" yWindow="2892"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>world</t>
-  </si>
-  <si>
-    <t>discount</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
-    <t>valueSum</t>
-  </si>
-  <si>
-    <t>avgValue</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -68,24 +43,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -351,49 +385,399 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.3125" customWidth="1"/>
-    <col min="2" max="2" width="7.3125" customWidth="1"/>
-    <col min="3" max="3" width="6.89453125" customWidth="1"/>
-    <col min="4" max="4" width="10.05078125" customWidth="1"/>
-    <col min="5" max="5" width="8.41796875" customWidth="1"/>
-    <col min="6" max="6" width="12.7890625" customWidth="1"/>
-    <col min="7" max="7" width="10.68359375" customWidth="1"/>
-    <col min="8" max="8" width="15.5234375" customWidth="1"/>
-    <col min="9" max="9" width="13.5234375" customWidth="1"/>
-    <col min="10" max="10" width="14.20703125" customWidth="1"/>
-    <col min="11" max="11" width="13.83984375" customWidth="1"/>
-    <col min="12" max="12" width="15.5234375" customWidth="1"/>
-    <col min="13" max="13" width="14.1015625" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="5.3125"/>
+    <col customWidth="1" max="2" min="2" width="7.3125"/>
+    <col customWidth="1" max="3" min="3" width="6.89453125"/>
+    <col customWidth="1" max="4" min="4" width="10.05078125"/>
+    <col customWidth="1" max="5" min="5" width="8.41796875"/>
+    <col customWidth="1" max="6" min="6" width="12.7890625"/>
+    <col customWidth="1" max="7" min="7" width="10.68359375"/>
+    <col customWidth="1" max="8" min="8" width="15.5234375"/>
+    <col customWidth="1" max="9" min="9" width="13.5234375"/>
+    <col customWidth="1" max="10" min="10" width="14.20703125"/>
+    <col customWidth="1" max="11" min="11" width="13.83984375"/>
+    <col customWidth="1" max="12" min="12" width="15.5234375"/>
+    <col customWidth="1" max="13" min="13" width="14.1015625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>world</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>valueSum</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>avgValue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-15.44752000000001</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-1.287</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-15.344</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-15.344</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-15.344</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-15.344</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-15.1326613</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-1.261</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-15.344</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-8.648136328750445</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-0.721</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-7.154114500802587</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-0.596</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-15.6712</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-1.306</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-15.35960000000001</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-1.280</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-15.344</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-7.44237014203806</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-0.620</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>navigation</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-9.778562613804493</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-0.815</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Computed known results for the wumpus world 2. Computed last results for world 2
</commit_message>
<xml_diff>
--- a/results/WorldKnown/ValueSum.xlsx
+++ b/results/WorldKnown/ValueSum.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="A2:E2"/>
@@ -776,6 +776,342 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D18" t="n">
+        <v>58.09999999999992</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0.182</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>58.09999999999992</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0.182</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D20" t="n">
+        <v>58.09999999999992</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.182</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>58.09999999999992</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.182</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D22" t="n">
+        <v>65.20874699999997</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.204</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>64.52430000000004</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0.202</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>161.46824210875</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0.505</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>151.7745720625</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0.474</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D28" t="n">
+        <v>165.5361683904909</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0.517</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D29" t="n">
+        <v>141.6811737500001</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0.443</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3011.463534858126</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>9.411</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3050.369902380611</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>9.532</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3028.382329004643</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>9.464</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>wumpus</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3046.927929267263</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>9.522</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>

</xml_diff>